<commit_message>
examples until addon technology added
</commit_message>
<xml_diff>
--- a/westeros_tutorial/input/Parameter_Demand.xlsx
+++ b/westeros_tutorial/input/Parameter_Demand.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/MESSAGE-China/projects/westeros_baseline/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/message_westeros/westeros_tutorial/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0128C495-AEF4-F945-963C-E36AE19DC169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139E3426-CF05-8C43-ABB8-BDFB6EDD070A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3920" yWindow="-21100" windowWidth="30240" windowHeight="17360" xr2:uid="{6A43CB06-E55E-0F45-9223-72CF49A70756}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{6A43CB06-E55E-0F45-9223-72CF49A70756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>